<commit_message>
Process 2 (Main) Updated
- Small Bug Fixes
- Added Extensive Reporting
- Added More Log Messages
- Added Extra Try Catch, to reduce errors
</commit_message>
<xml_diff>
--- a/Project (UiPath)/ToborInc-Files/ArticleArchive.xlsx
+++ b/Project (UiPath)/ToborInc-Files/ArticleArchive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA Workspace\SFIA Project 2\Project (UiPath)\ToborInc-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0ABC627-ECF0-4B84-9478-4D482810D56B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF34518D-7E2C-45AE-9B38-6D0DA1754E8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arcive" sheetId="2" r:id="rId1"/>
@@ -26,18 +26,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>URL</t>
   </si>
   <si>
+    <t>https://gadgets.ndtv.com/apps/news/zomato-employees-burn-company-t-shirts-to-protest-chinese-investment-in-firm-2253507</t>
+  </si>
+  <si>
     <t>https://www.bbc.co.uk/news/business-53214291</t>
   </si>
   <si>
     <t>https://www.wired.co.uk/article/apple-bmw-uwb-car-key</t>
   </si>
   <si>
-    <t>https://gadgets.ndtv.com/apps/news/zomato-employees-burn-company-t-shirts-to-protest-chinese-investment-in-firm-2253507</t>
+    <t>https://gadgets.ndtv.com/mobiles/news/oneplus-8-pro-sale-india-today-june-29-price-rs-54989-specifications-amazon-offer-2253327</t>
   </si>
   <si>
     <t>https://www.skysports.com/golf/news/12176/12017150/dylan-frittelli-becomes-fourth-pga-tour-player-to-test-positive-for-covid-19</t>
@@ -47,6 +50,15 @@
   </si>
   <si>
     <t>https://uk.reuters.com/article/uk-soccer-england-new-mci-report/holders-manchester-city-cruise-past-newcastle-into-fa-cup-semis-idUKKBN23Z0RS</t>
+  </si>
+  <si>
+    <t>https://www.entrepreneur.com/article/347406</t>
+  </si>
+  <si>
+    <t>https://www.bbc.co.uk/news/entertainment-arts-53190585</t>
+  </si>
+  <si>
+    <t>https://news.sky.com/story/molly-conlin-former-eastenders-star-held-at-knifepoint-by-robbers-who-broke-into-her-home-12017105</t>
   </si>
 </sst>
 </file>
@@ -372,7 +384,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -382,10 +394,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,32 +412,47 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>